<commit_message>
Copy US files for 3.3 updates
</commit_message>
<xml_diff>
--- a/InputData/endo-learn/PDiBCpDoC/Perc Decline in Battery Cost per Doubling of Cap.xlsx
+++ b/InputData/endo-learn/PDiBCpDoC/Perc Decline in Battery Cost per Doubling of Cap.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\endo-learn\PDiBCpDoC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\endo-learn\PDiBCpDoC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D81FD32-760B-4369-A9B7-97CB22806FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="22035" windowHeight="11835"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="PDiBCpDoC" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -31,28 +43,28 @@
     <t>PDiBCpDoC Perc Decline in Battery Cost per Doubling of Capacity</t>
   </si>
   <si>
-    <t>Bloomberg New Energy Finance</t>
-  </si>
-  <si>
-    <t>New Energy Outlook 2018</t>
-  </si>
-  <si>
-    <t>https://bnef.turtl.co/story/neo2018</t>
-  </si>
-  <si>
-    <t>Chapter 6, Page 2, Figure at bottom of column 2 (online), also reproduced below</t>
-  </si>
-  <si>
-    <t>Note that the graph only extends to 2030, not 2050</t>
-  </si>
-  <si>
     <t>Perc Decline per Doubling (dimensionless)</t>
+  </si>
+  <si>
+    <t>https://pubs.rsc.org/en/content/articlepdf/2021/ee/d0ee02681f?page=search</t>
+  </si>
+  <si>
+    <t>Re-examining rates of lithium-ion battery technology improvement and cost decline</t>
+  </si>
+  <si>
+    <t>Massachusetts Institute of Technology</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>Note: We take the average of learning rates quoted in the Abstract (20%-27%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,55 +132,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>29286</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="1524000"/>
-          <a:ext cx="10058400" cy="6506286"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -247,6 +210,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -282,6 +262,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -457,85 +454,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C8" s="3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.1328125" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.18</v>
+        <f>AVERAGE(0.2,0.27)</f>
+        <v>0.23500000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>